<commit_message>
added files on exports tasks
</commit_message>
<xml_diff>
--- a/public/assets/sample_one.xlsx
+++ b/public/assets/sample_one.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albogast\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\steam\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2797AA04-61A5-40F1-97C6-55741852C34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>DED - MERU</t>
   </si>
@@ -203,12 +193,18 @@
   </si>
   <si>
     <t>Mussa Hassan</t>
+  </si>
+  <si>
+    <t>nextkin</t>
+  </si>
+  <si>
+    <t>kinphone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -308,7 +304,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -661,25 +657,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -707,8 +703,14 @@
       <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
@@ -734,8 +736,10 @@
         <v>49</v>
       </c>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -761,8 +765,10 @@
         <v>49</v>
       </c>
       <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -788,8 +794,10 @@
         <v>49</v>
       </c>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -815,8 +823,10 @@
         <v>49</v>
       </c>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -842,8 +852,10 @@
         <v>49</v>
       </c>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -869,8 +881,10 @@
         <v>49</v>
       </c>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -896,8 +910,10 @@
         <v>49</v>
       </c>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -923,8 +939,10 @@
         <v>49</v>
       </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -950,8 +968,10 @@
         <v>49</v>
       </c>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -977,8 +997,10 @@
         <v>49</v>
       </c>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1004,8 +1026,10 @@
         <v>49</v>
       </c>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
@@ -1031,8 +1055,10 @@
         <v>49</v>
       </c>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
@@ -1058,12 +1084,14 @@
         <v>49</v>
       </c>
       <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C14">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:J14">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A13">

</xml_diff>

<commit_message>
added new files of report expoerts
</commit_message>
<xml_diff>
--- a/public/assets/sample_one.xlsx
+++ b/public/assets/sample_one.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\steam\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2797AA04-61A5-40F1-97C6-55741852C34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0708CF5F-B5B0-4F1C-AE55-313F0B7A3D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>DED - MERU</t>
   </si>
@@ -199,6 +208,12 @@
   </si>
   <si>
     <t>kinphone</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>nextaction</t>
   </si>
 </sst>
 </file>
@@ -658,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,10 +687,10 @@
     <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.26953125" customWidth="1"/>
+    <col min="8" max="12" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -704,13 +719,19 @@
         <v>47</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
@@ -738,8 +759,10 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -767,8 +790,10 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -796,8 +821,10 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -825,8 +852,10 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -854,8 +883,10 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -883,8 +914,10 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -912,8 +945,10 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -941,8 +976,10 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -970,8 +1007,10 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -999,8 +1038,10 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1028,8 +1069,10 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
@@ -1057,8 +1100,10 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
@@ -1086,12 +1131,14 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C14">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:J14">
+  <conditionalFormatting sqref="H2:L14">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A13">

</xml_diff>